<commit_message>
Now we got RouteConfig class for each screen vue component! TODO: Create Array List of RouteConfigs.
</commit_message>
<xml_diff>
--- a/meta/program/BlancoVueComponentResourceBundle.xlsx
+++ b/meta/program/BlancoVueComponentResourceBundle.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tueda/data/webstorm/blanco/blancoVueComponent/meta/program/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F379FEBF-1C5B-FE4D-A3B9-8EE0E7E3FD4D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29452314-2424-3547-BA20-B9B715251C6C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="9600" yWindow="460" windowWidth="28800" windowHeight="17540" tabRatio="860" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="122">
   <si>
     <t>説明</t>
     <rPh sb="0" eb="2">
@@ -650,6 +650,25 @@
   <si>
     <t>blancovuecomponent-header-interface</t>
     <phoneticPr fontId="5"/>
+  </si>
+  <si>
+    <t>XML2SOURCE_FILE.ROUTECONFIG.PARAMETER</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>XML2SOURCE_FILE.ROUTECONFIG.CLASS</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>RouteConfigのパラメータです: [{0}]。</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>RouteConfigを定義します: [{0}]。</t>
+    <rPh sb="12" eb="14">
+      <t>テイギシマス</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
   </si>
 </sst>
 </file>
@@ -1601,10 +1620,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:I91"/>
+  <dimension ref="A1:I93"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="C34" sqref="C34"/>
+    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
+      <selection activeCell="C80" sqref="C80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14"/>
@@ -1771,7 +1790,7 @@
     </row>
     <row r="17" spans="1:9">
       <c r="A17" s="28">
-        <f t="shared" ref="A17:A83" si="0">A16+1</f>
+        <f t="shared" ref="A17:A85" si="0">A16+1</f>
         <v>3</v>
       </c>
       <c r="B17" s="23"/>
@@ -2218,7 +2237,7 @@
     </row>
     <row r="47" spans="1:9">
       <c r="A47" s="36">
-        <f t="shared" si="0"/>
+        <f>A46+1</f>
         <v>33</v>
       </c>
       <c r="B47" s="23"/>
@@ -2697,9 +2716,11 @@
         <f t="shared" si="0"/>
         <v>65</v>
       </c>
-      <c r="B79" s="23"/>
+      <c r="B79" s="23" t="s">
+        <v>119</v>
+      </c>
       <c r="C79" s="20" t="s">
-        <v>72</v>
+        <v>121</v>
       </c>
       <c r="D79" s="21"/>
       <c r="E79" s="21"/>
@@ -2711,9 +2732,11 @@
         <f t="shared" si="0"/>
         <v>66</v>
       </c>
-      <c r="B80" s="23"/>
+      <c r="B80" s="23" t="s">
+        <v>118</v>
+      </c>
       <c r="C80" s="20" t="s">
-        <v>88</v>
+        <v>120</v>
       </c>
       <c r="D80" s="21"/>
       <c r="E80" s="21"/>
@@ -2722,8 +2745,8 @@
     </row>
     <row r="81" spans="1:7">
       <c r="A81" s="36">
-        <f t="shared" si="0"/>
-        <v>67</v>
+        <f>A78+1</f>
+        <v>65</v>
       </c>
       <c r="B81" s="23"/>
       <c r="C81" s="20" t="s">
@@ -2737,13 +2760,11 @@
     <row r="82" spans="1:7">
       <c r="A82" s="36">
         <f t="shared" si="0"/>
-        <v>68</v>
-      </c>
-      <c r="B82" s="23" t="s">
-        <v>97</v>
-      </c>
+        <v>66</v>
+      </c>
+      <c r="B82" s="23"/>
       <c r="C82" s="20" t="s">
-        <v>98</v>
+        <v>88</v>
       </c>
       <c r="D82" s="21"/>
       <c r="E82" s="21"/>
@@ -2753,13 +2774,11 @@
     <row r="83" spans="1:7">
       <c r="A83" s="36">
         <f t="shared" si="0"/>
-        <v>69</v>
-      </c>
-      <c r="B83" s="23" t="s">
-        <v>99</v>
-      </c>
+        <v>67</v>
+      </c>
+      <c r="B83" s="23"/>
       <c r="C83" s="20" t="s">
-        <v>100</v>
+        <v>72</v>
       </c>
       <c r="D83" s="21"/>
       <c r="E83" s="21"/>
@@ -2768,14 +2787,14 @@
     </row>
     <row r="84" spans="1:7">
       <c r="A84" s="36">
-        <f t="shared" ref="A84:A89" si="1">A83+1</f>
-        <v>70</v>
+        <f t="shared" si="0"/>
+        <v>68</v>
       </c>
       <c r="B84" s="23" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="C84" s="20" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="D84" s="21"/>
       <c r="E84" s="21"/>
@@ -2784,14 +2803,14 @@
     </row>
     <row r="85" spans="1:7">
       <c r="A85" s="36">
-        <f t="shared" si="1"/>
-        <v>71</v>
+        <f t="shared" si="0"/>
+        <v>69</v>
       </c>
       <c r="B85" s="23" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="C85" s="20" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="D85" s="21"/>
       <c r="E85" s="21"/>
@@ -2800,14 +2819,14 @@
     </row>
     <row r="86" spans="1:7">
       <c r="A86" s="36">
-        <f t="shared" si="1"/>
-        <v>72</v>
+        <f t="shared" ref="A86:A91" si="1">A85+1</f>
+        <v>70</v>
       </c>
       <c r="B86" s="23" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="C86" s="20" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="D86" s="21"/>
       <c r="E86" s="21"/>
@@ -2817,13 +2836,13 @@
     <row r="87" spans="1:7">
       <c r="A87" s="36">
         <f t="shared" si="1"/>
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B87" s="23" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="C87" s="20" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="D87" s="21"/>
       <c r="E87" s="21"/>
@@ -2833,13 +2852,13 @@
     <row r="88" spans="1:7">
       <c r="A88" s="36">
         <f t="shared" si="1"/>
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B88" s="23" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="C88" s="20" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="D88" s="21"/>
       <c r="E88" s="21"/>
@@ -2849,13 +2868,13 @@
     <row r="89" spans="1:7">
       <c r="A89" s="36">
         <f t="shared" si="1"/>
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B89" s="23" t="s">
-        <v>89</v>
+        <v>107</v>
       </c>
       <c r="C89" s="20" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="D89" s="21"/>
       <c r="E89" s="21"/>
@@ -2863,22 +2882,54 @@
       <c r="G89" s="22"/>
     </row>
     <row r="90" spans="1:7">
-      <c r="A90" s="28"/>
-      <c r="B90" s="23"/>
-      <c r="C90" s="20"/>
-      <c r="D90" s="34"/>
-      <c r="E90" s="34"/>
-      <c r="F90" s="34"/>
-      <c r="G90" s="35"/>
+      <c r="A90" s="36">
+        <f t="shared" si="1"/>
+        <v>74</v>
+      </c>
+      <c r="B90" s="23" t="s">
+        <v>109</v>
+      </c>
+      <c r="C90" s="20" t="s">
+        <v>110</v>
+      </c>
+      <c r="D90" s="21"/>
+      <c r="E90" s="21"/>
+      <c r="F90" s="21"/>
+      <c r="G90" s="22"/>
     </row>
     <row r="91" spans="1:7">
-      <c r="A91" s="29"/>
-      <c r="B91" s="24"/>
-      <c r="C91" s="25"/>
-      <c r="D91" s="26"/>
-      <c r="E91" s="26"/>
-      <c r="F91" s="26"/>
-      <c r="G91" s="27"/>
+      <c r="A91" s="36">
+        <f t="shared" si="1"/>
+        <v>75</v>
+      </c>
+      <c r="B91" s="23" t="s">
+        <v>89</v>
+      </c>
+      <c r="C91" s="20" t="s">
+        <v>111</v>
+      </c>
+      <c r="D91" s="21"/>
+      <c r="E91" s="21"/>
+      <c r="F91" s="21"/>
+      <c r="G91" s="22"/>
+    </row>
+    <row r="92" spans="1:7">
+      <c r="A92" s="28"/>
+      <c r="B92" s="23"/>
+      <c r="C92" s="20"/>
+      <c r="D92" s="34"/>
+      <c r="E92" s="34"/>
+      <c r="F92" s="34"/>
+      <c r="G92" s="35"/>
+    </row>
+    <row r="93" spans="1:7">
+      <c r="A93" s="29"/>
+      <c r="B93" s="24"/>
+      <c r="C93" s="25"/>
+      <c r="D93" s="26"/>
+      <c r="E93" s="26"/>
+      <c r="F93" s="26"/>
+      <c r="G93" s="27"/>
     </row>
   </sheetData>
   <mergeCells count="3">

</xml_diff>

<commit_message>
1.0.4: Make RequestFactory to Interface.
</commit_message>
<xml_diff>
--- a/meta/program/BlancoVueComponentResourceBundle.xlsx
+++ b/meta/program/BlancoVueComponentResourceBundle.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tueda/data/webstorm/blanco/blancoVueComponent/meta/program/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F7905BE-DB28-1643-9286-70FEB43A8430}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46A3D74F-1874-A14F-8365-2685FAEE6F6F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="9600" yWindow="500" windowWidth="28800" windowHeight="17540" tabRatio="860" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="148">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="150">
   <si>
     <t>説明</t>
     <rPh sb="0" eb="2">
@@ -813,6 +813,17 @@
     <t>{0} クラスを生成します。</t>
     <rPh sb="8" eb="10">
       <t xml:space="preserve">セイセイ </t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>XML2SOURCE_FILE.REQUEST_FACTORY_RETURN.DESCRIPTION</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>{0} クラスを返却します。</t>
+    <rPh sb="8" eb="10">
+      <t xml:space="preserve">ヘンキャク </t>
     </rPh>
     <phoneticPr fontId="1"/>
   </si>
@@ -1748,10 +1759,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:I113"/>
+  <dimension ref="A1:I114"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A76" workbookViewId="0">
-      <selection activeCell="C99" sqref="C99"/>
+    <sheetView tabSelected="1" topLeftCell="A69" workbookViewId="0">
+      <selection activeCell="C100" sqref="C100"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14"/>
@@ -2872,7 +2883,7 @@
     </row>
     <row r="81" spans="1:7">
       <c r="A81" s="28">
-        <f t="shared" ref="A81:A111" si="1">A80+1</f>
+        <f t="shared" ref="A81:A112" si="1">A80+1</f>
         <v>67</v>
       </c>
       <c r="B81" s="23" t="s">
@@ -3155,8 +3166,12 @@
         <f t="shared" si="1"/>
         <v>85</v>
       </c>
-      <c r="B99" s="23"/>
-      <c r="C99" s="20"/>
+      <c r="B99" s="23" t="s">
+        <v>148</v>
+      </c>
+      <c r="C99" s="20" t="s">
+        <v>149</v>
+      </c>
       <c r="D99" s="21"/>
       <c r="E99" s="21"/>
       <c r="F99" s="21"/>
@@ -3180,9 +3195,7 @@
         <v>87</v>
       </c>
       <c r="B101" s="23"/>
-      <c r="C101" s="20" t="s">
-        <v>69</v>
-      </c>
+      <c r="C101" s="20"/>
       <c r="D101" s="21"/>
       <c r="E101" s="21"/>
       <c r="F101" s="21"/>
@@ -3195,7 +3208,7 @@
       </c>
       <c r="B102" s="23"/>
       <c r="C102" s="20" t="s">
-        <v>85</v>
+        <v>69</v>
       </c>
       <c r="D102" s="21"/>
       <c r="E102" s="21"/>
@@ -3209,7 +3222,7 @@
       </c>
       <c r="B103" s="23"/>
       <c r="C103" s="20" t="s">
-        <v>69</v>
+        <v>85</v>
       </c>
       <c r="D103" s="21"/>
       <c r="E103" s="21"/>
@@ -3221,11 +3234,9 @@
         <f t="shared" si="1"/>
         <v>90</v>
       </c>
-      <c r="B104" s="23" t="s">
-        <v>91</v>
-      </c>
+      <c r="B104" s="23"/>
       <c r="C104" s="20" t="s">
-        <v>92</v>
+        <v>69</v>
       </c>
       <c r="D104" s="21"/>
       <c r="E104" s="21"/>
@@ -3238,10 +3249,10 @@
         <v>91</v>
       </c>
       <c r="B105" s="23" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C105" s="20" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="D105" s="21"/>
       <c r="E105" s="21"/>
@@ -3254,10 +3265,10 @@
         <v>92</v>
       </c>
       <c r="B106" s="23" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C106" s="20" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="D106" s="21"/>
       <c r="E106" s="21"/>
@@ -3270,10 +3281,10 @@
         <v>93</v>
       </c>
       <c r="B107" s="23" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C107" s="20" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="D107" s="21"/>
       <c r="E107" s="21"/>
@@ -3286,10 +3297,10 @@
         <v>94</v>
       </c>
       <c r="B108" s="23" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C108" s="20" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="D108" s="21"/>
       <c r="E108" s="21"/>
@@ -3302,10 +3313,10 @@
         <v>95</v>
       </c>
       <c r="B109" s="23" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C109" s="20" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="D109" s="21"/>
       <c r="E109" s="21"/>
@@ -3318,10 +3329,10 @@
         <v>96</v>
       </c>
       <c r="B110" s="23" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C110" s="20" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="D110" s="21"/>
       <c r="E110" s="21"/>
@@ -3334,10 +3345,10 @@
         <v>97</v>
       </c>
       <c r="B111" s="23" t="s">
-        <v>86</v>
+        <v>103</v>
       </c>
       <c r="C111" s="20" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D111" s="21"/>
       <c r="E111" s="21"/>
@@ -3345,22 +3356,38 @@
       <c r="G111" s="22"/>
     </row>
     <row r="112" spans="1:7">
-      <c r="A112" s="28"/>
-      <c r="B112" s="23"/>
-      <c r="C112" s="20"/>
-      <c r="D112" s="34"/>
-      <c r="E112" s="34"/>
-      <c r="F112" s="34"/>
-      <c r="G112" s="35"/>
+      <c r="A112" s="28">
+        <f t="shared" si="1"/>
+        <v>98</v>
+      </c>
+      <c r="B112" s="23" t="s">
+        <v>86</v>
+      </c>
+      <c r="C112" s="20" t="s">
+        <v>105</v>
+      </c>
+      <c r="D112" s="21"/>
+      <c r="E112" s="21"/>
+      <c r="F112" s="21"/>
+      <c r="G112" s="22"/>
     </row>
     <row r="113" spans="1:7">
-      <c r="A113" s="29"/>
-      <c r="B113" s="24"/>
-      <c r="C113" s="25"/>
-      <c r="D113" s="26"/>
-      <c r="E113" s="26"/>
-      <c r="F113" s="26"/>
-      <c r="G113" s="27"/>
+      <c r="A113" s="28"/>
+      <c r="B113" s="23"/>
+      <c r="C113" s="20"/>
+      <c r="D113" s="34"/>
+      <c r="E113" s="34"/>
+      <c r="F113" s="34"/>
+      <c r="G113" s="35"/>
+    </row>
+    <row r="114" spans="1:7">
+      <c r="A114" s="29"/>
+      <c r="B114" s="24"/>
+      <c r="C114" s="25"/>
+      <c r="D114" s="26"/>
+      <c r="E114" s="26"/>
+      <c r="F114" s="26"/>
+      <c r="G114" s="27"/>
     </row>
   </sheetData>
   <mergeCells count="3">

</xml_diff>

<commit_message>
1.0.8: Add componentId to component props.
</commit_message>
<xml_diff>
--- a/meta/program/BlancoVueComponentResourceBundle.xlsx
+++ b/meta/program/BlancoVueComponentResourceBundle.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tueda/data/webstorm/blanco/blancoVueComponent/meta/program/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46A3D74F-1874-A14F-8365-2685FAEE6F6F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4B6AF1C-2981-E946-AF9D-31D9BF6BB434}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="9600" yWindow="500" windowWidth="28800" windowHeight="17540" tabRatio="860" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="150">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="152">
   <si>
     <t>説明</t>
     <rPh sb="0" eb="2">
@@ -825,6 +825,14 @@
     <rPh sb="8" eb="10">
       <t xml:space="preserve">ヘンキャク </t>
     </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>XML2SOURCE_FILE.PROPS_COMPOENENT_ID.DESCRIPTION</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>コンポーネントのcomponentIdプロパティです</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -1759,10 +1767,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:I114"/>
+  <dimension ref="A1:I115"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A69" workbookViewId="0">
-      <selection activeCell="C100" sqref="C100"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14"/>
@@ -2883,7 +2891,7 @@
     </row>
     <row r="81" spans="1:7">
       <c r="A81" s="28">
-        <f t="shared" ref="A81:A112" si="1">A80+1</f>
+        <f t="shared" ref="A81:A113" si="1">A80+1</f>
         <v>67</v>
       </c>
       <c r="B81" s="23" t="s">
@@ -3039,10 +3047,10 @@
         <v>77</v>
       </c>
       <c r="B91" s="23" t="s">
-        <v>128</v>
+        <v>150</v>
       </c>
       <c r="C91" s="20" t="s">
-        <v>131</v>
+        <v>151</v>
       </c>
       <c r="D91" s="21"/>
       <c r="E91" s="21"/>
@@ -3055,10 +3063,10 @@
         <v>78</v>
       </c>
       <c r="B92" s="23" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="C92" s="20" t="s">
-        <v>138</v>
+        <v>131</v>
       </c>
       <c r="D92" s="21"/>
       <c r="E92" s="21"/>
@@ -3071,10 +3079,10 @@
         <v>79</v>
       </c>
       <c r="B93" s="23" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C93" s="20" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D93" s="21"/>
       <c r="E93" s="21"/>
@@ -3087,10 +3095,10 @@
         <v>80</v>
       </c>
       <c r="B94" s="23" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C94" s="20" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
       <c r="D94" s="21"/>
       <c r="E94" s="21"/>
@@ -3103,10 +3111,10 @@
         <v>81</v>
       </c>
       <c r="B95" s="23" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C95" s="20" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D95" s="21"/>
       <c r="E95" s="21"/>
@@ -3119,10 +3127,10 @@
         <v>82</v>
       </c>
       <c r="B96" s="23" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="C96" s="20" t="s">
-        <v>143</v>
+        <v>137</v>
       </c>
       <c r="D96" s="21"/>
       <c r="E96" s="21"/>
@@ -3135,10 +3143,10 @@
         <v>83</v>
       </c>
       <c r="B97" s="23" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C97" s="20" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="D97" s="21"/>
       <c r="E97" s="21"/>
@@ -3151,10 +3159,10 @@
         <v>84</v>
       </c>
       <c r="B98" s="23" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="C98" s="20" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="D98" s="21"/>
       <c r="E98" s="21"/>
@@ -3167,10 +3175,10 @@
         <v>85</v>
       </c>
       <c r="B99" s="23" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="C99" s="20" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="D99" s="21"/>
       <c r="E99" s="21"/>
@@ -3182,8 +3190,12 @@
         <f t="shared" si="1"/>
         <v>86</v>
       </c>
-      <c r="B100" s="23"/>
-      <c r="C100" s="20"/>
+      <c r="B100" s="23" t="s">
+        <v>148</v>
+      </c>
+      <c r="C100" s="20" t="s">
+        <v>149</v>
+      </c>
       <c r="D100" s="21"/>
       <c r="E100" s="21"/>
       <c r="F100" s="21"/>
@@ -3207,9 +3219,7 @@
         <v>88</v>
       </c>
       <c r="B102" s="23"/>
-      <c r="C102" s="20" t="s">
-        <v>69</v>
-      </c>
+      <c r="C102" s="20"/>
       <c r="D102" s="21"/>
       <c r="E102" s="21"/>
       <c r="F102" s="21"/>
@@ -3222,7 +3232,7 @@
       </c>
       <c r="B103" s="23"/>
       <c r="C103" s="20" t="s">
-        <v>85</v>
+        <v>69</v>
       </c>
       <c r="D103" s="21"/>
       <c r="E103" s="21"/>
@@ -3236,7 +3246,7 @@
       </c>
       <c r="B104" s="23"/>
       <c r="C104" s="20" t="s">
-        <v>69</v>
+        <v>85</v>
       </c>
       <c r="D104" s="21"/>
       <c r="E104" s="21"/>
@@ -3248,11 +3258,9 @@
         <f t="shared" si="1"/>
         <v>91</v>
       </c>
-      <c r="B105" s="23" t="s">
-        <v>91</v>
-      </c>
+      <c r="B105" s="23"/>
       <c r="C105" s="20" t="s">
-        <v>92</v>
+        <v>69</v>
       </c>
       <c r="D105" s="21"/>
       <c r="E105" s="21"/>
@@ -3265,10 +3273,10 @@
         <v>92</v>
       </c>
       <c r="B106" s="23" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C106" s="20" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="D106" s="21"/>
       <c r="E106" s="21"/>
@@ -3281,10 +3289,10 @@
         <v>93</v>
       </c>
       <c r="B107" s="23" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C107" s="20" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="D107" s="21"/>
       <c r="E107" s="21"/>
@@ -3297,10 +3305,10 @@
         <v>94</v>
       </c>
       <c r="B108" s="23" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C108" s="20" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="D108" s="21"/>
       <c r="E108" s="21"/>
@@ -3313,10 +3321,10 @@
         <v>95</v>
       </c>
       <c r="B109" s="23" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C109" s="20" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="D109" s="21"/>
       <c r="E109" s="21"/>
@@ -3329,10 +3337,10 @@
         <v>96</v>
       </c>
       <c r="B110" s="23" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C110" s="20" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="D110" s="21"/>
       <c r="E110" s="21"/>
@@ -3345,10 +3353,10 @@
         <v>97</v>
       </c>
       <c r="B111" s="23" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C111" s="20" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="D111" s="21"/>
       <c r="E111" s="21"/>
@@ -3361,10 +3369,10 @@
         <v>98</v>
       </c>
       <c r="B112" s="23" t="s">
-        <v>86</v>
+        <v>103</v>
       </c>
       <c r="C112" s="20" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D112" s="21"/>
       <c r="E112" s="21"/>
@@ -3372,22 +3380,38 @@
       <c r="G112" s="22"/>
     </row>
     <row r="113" spans="1:7">
-      <c r="A113" s="28"/>
-      <c r="B113" s="23"/>
-      <c r="C113" s="20"/>
-      <c r="D113" s="34"/>
-      <c r="E113" s="34"/>
-      <c r="F113" s="34"/>
-      <c r="G113" s="35"/>
+      <c r="A113" s="28">
+        <f t="shared" si="1"/>
+        <v>99</v>
+      </c>
+      <c r="B113" s="23" t="s">
+        <v>86</v>
+      </c>
+      <c r="C113" s="20" t="s">
+        <v>105</v>
+      </c>
+      <c r="D113" s="21"/>
+      <c r="E113" s="21"/>
+      <c r="F113" s="21"/>
+      <c r="G113" s="22"/>
     </row>
     <row r="114" spans="1:7">
-      <c r="A114" s="29"/>
-      <c r="B114" s="24"/>
-      <c r="C114" s="25"/>
-      <c r="D114" s="26"/>
-      <c r="E114" s="26"/>
-      <c r="F114" s="26"/>
-      <c r="G114" s="27"/>
+      <c r="A114" s="28"/>
+      <c r="B114" s="23"/>
+      <c r="C114" s="20"/>
+      <c r="D114" s="34"/>
+      <c r="E114" s="34"/>
+      <c r="F114" s="34"/>
+      <c r="G114" s="35"/>
+    </row>
+    <row r="115" spans="1:7">
+      <c r="A115" s="29"/>
+      <c r="B115" s="24"/>
+      <c r="C115" s="25"/>
+      <c r="D115" s="26"/>
+      <c r="E115" s="26"/>
+      <c r="F115" s="26"/>
+      <c r="G115" s="27"/>
     </row>
   </sheetData>
   <mergeCells count="3">

</xml_diff>

<commit_message>
3.0.12: Add children property to MenuItemInterface.
</commit_message>
<xml_diff>
--- a/meta/program/BlancoVueComponentResourceBundle.xlsx
+++ b/meta/program/BlancoVueComponentResourceBundle.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10714"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tueda/data/webstorm/blanco/blancoVueComponent/meta/program/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75CF0984-3514-2B46-9247-32056DBD90AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE957C3A-CADD-F64C-8C7C-05A8255A937A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22380" yWindow="5160" windowWidth="28800" windowHeight="17540" tabRatio="860" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6660" yWindow="10080" windowWidth="28800" windowHeight="17540" tabRatio="860" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ja" sheetId="9" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="176">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="178">
   <si>
     <t>説明</t>
     <rPh sb="0" eb="2">
@@ -970,6 +970,17 @@
     <t>MenuItem を定義します。[ {0} ]</t>
     <rPh sb="10" eb="12">
       <t xml:space="preserve">テイギ </t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>XML2SOURCE_FILE.MENU.ITEM.CHILDREN</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>メニューノードの子階層です。</t>
+    <rPh sb="8" eb="11">
+      <t xml:space="preserve">コカイソウ </t>
     </rPh>
     <phoneticPr fontId="1"/>
   </si>
@@ -1903,10 +1914,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:I128"/>
+  <dimension ref="A1:I129"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A79" workbookViewId="0">
-      <selection activeCell="C113" sqref="C113"/>
+      <selection activeCell="C114" sqref="C114"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14"/>
@@ -3029,7 +3040,7 @@
     </row>
     <row r="81" spans="1:7">
       <c r="A81" s="27">
-        <f t="shared" ref="A81:A126" si="1">A80+1</f>
+        <f t="shared" ref="A81:A127" si="1">A80+1</f>
         <v>67</v>
       </c>
       <c r="B81" s="22" t="s">
@@ -3513,8 +3524,8 @@
     </row>
     <row r="112" spans="1:7">
       <c r="A112" s="27">
-        <f>A110+1</f>
-        <v>97</v>
+        <f>A109+1</f>
+        <v>96</v>
       </c>
       <c r="B112" s="22" t="s">
         <v>171</v>
@@ -3529,14 +3540,14 @@
     </row>
     <row r="113" spans="1:7">
       <c r="A113" s="27">
-        <f>A111+1</f>
-        <v>98</v>
+        <f>A110+1</f>
+        <v>97</v>
       </c>
       <c r="B113" s="22" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="C113" s="19" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="D113" s="20"/>
       <c r="E113" s="20"/>
@@ -3545,11 +3556,15 @@
     </row>
     <row r="114" spans="1:7">
       <c r="A114" s="27">
-        <f t="shared" si="1"/>
-        <v>99</v>
-      </c>
-      <c r="B114" s="22"/>
-      <c r="C114" s="19"/>
+        <f>A111+1</f>
+        <v>98</v>
+      </c>
+      <c r="B114" s="22" t="s">
+        <v>174</v>
+      </c>
+      <c r="C114" s="19" t="s">
+        <v>175</v>
+      </c>
       <c r="D114" s="20"/>
       <c r="E114" s="20"/>
       <c r="F114" s="20"/>
@@ -3558,7 +3573,7 @@
     <row r="115" spans="1:7">
       <c r="A115" s="27">
         <f t="shared" si="1"/>
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B115" s="22"/>
       <c r="C115" s="19"/>
@@ -3570,12 +3585,10 @@
     <row r="116" spans="1:7">
       <c r="A116" s="27">
         <f t="shared" si="1"/>
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B116" s="22"/>
-      <c r="C116" s="19" t="s">
-        <v>69</v>
-      </c>
+      <c r="C116" s="19"/>
       <c r="D116" s="20"/>
       <c r="E116" s="20"/>
       <c r="F116" s="20"/>
@@ -3584,11 +3597,11 @@
     <row r="117" spans="1:7">
       <c r="A117" s="27">
         <f t="shared" si="1"/>
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B117" s="22"/>
       <c r="C117" s="19" t="s">
-        <v>85</v>
+        <v>69</v>
       </c>
       <c r="D117" s="20"/>
       <c r="E117" s="20"/>
@@ -3598,11 +3611,11 @@
     <row r="118" spans="1:7">
       <c r="A118" s="27">
         <f t="shared" si="1"/>
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B118" s="22"/>
       <c r="C118" s="19" t="s">
-        <v>69</v>
+        <v>85</v>
       </c>
       <c r="D118" s="20"/>
       <c r="E118" s="20"/>
@@ -3612,13 +3625,11 @@
     <row r="119" spans="1:7">
       <c r="A119" s="27">
         <f t="shared" si="1"/>
-        <v>104</v>
-      </c>
-      <c r="B119" s="22" t="s">
-        <v>91</v>
-      </c>
+        <v>103</v>
+      </c>
+      <c r="B119" s="22"/>
       <c r="C119" s="19" t="s">
-        <v>92</v>
+        <v>69</v>
       </c>
       <c r="D119" s="20"/>
       <c r="E119" s="20"/>
@@ -3628,13 +3639,13 @@
     <row r="120" spans="1:7">
       <c r="A120" s="27">
         <f t="shared" si="1"/>
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B120" s="22" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C120" s="19" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="D120" s="20"/>
       <c r="E120" s="20"/>
@@ -3644,13 +3655,13 @@
     <row r="121" spans="1:7">
       <c r="A121" s="27">
         <f t="shared" si="1"/>
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B121" s="22" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C121" s="19" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="D121" s="20"/>
       <c r="E121" s="20"/>
@@ -3660,13 +3671,13 @@
     <row r="122" spans="1:7">
       <c r="A122" s="27">
         <f t="shared" si="1"/>
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B122" s="22" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C122" s="19" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="D122" s="20"/>
       <c r="E122" s="20"/>
@@ -3676,13 +3687,13 @@
     <row r="123" spans="1:7">
       <c r="A123" s="27">
         <f t="shared" si="1"/>
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B123" s="22" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C123" s="19" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="D123" s="20"/>
       <c r="E123" s="20"/>
@@ -3692,13 +3703,13 @@
     <row r="124" spans="1:7">
       <c r="A124" s="27">
         <f t="shared" si="1"/>
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B124" s="22" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C124" s="19" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="D124" s="20"/>
       <c r="E124" s="20"/>
@@ -3708,13 +3719,13 @@
     <row r="125" spans="1:7">
       <c r="A125" s="27">
         <f t="shared" si="1"/>
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B125" s="22" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C125" s="19" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="D125" s="20"/>
       <c r="E125" s="20"/>
@@ -3724,13 +3735,13 @@
     <row r="126" spans="1:7">
       <c r="A126" s="27">
         <f t="shared" si="1"/>
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B126" s="22" t="s">
-        <v>86</v>
+        <v>103</v>
       </c>
       <c r="C126" s="19" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D126" s="20"/>
       <c r="E126" s="20"/>
@@ -3738,22 +3749,38 @@
       <c r="G126" s="21"/>
     </row>
     <row r="127" spans="1:7">
-      <c r="A127" s="27"/>
-      <c r="B127" s="22"/>
-      <c r="C127" s="19"/>
-      <c r="D127" s="32"/>
-      <c r="E127" s="32"/>
-      <c r="F127" s="32"/>
-      <c r="G127" s="33"/>
+      <c r="A127" s="27">
+        <f t="shared" si="1"/>
+        <v>111</v>
+      </c>
+      <c r="B127" s="22" t="s">
+        <v>86</v>
+      </c>
+      <c r="C127" s="19" t="s">
+        <v>105</v>
+      </c>
+      <c r="D127" s="20"/>
+      <c r="E127" s="20"/>
+      <c r="F127" s="20"/>
+      <c r="G127" s="21"/>
     </row>
     <row r="128" spans="1:7">
-      <c r="A128" s="28"/>
-      <c r="B128" s="23"/>
-      <c r="C128" s="24"/>
-      <c r="D128" s="25"/>
-      <c r="E128" s="25"/>
-      <c r="F128" s="25"/>
-      <c r="G128" s="26"/>
+      <c r="A128" s="27"/>
+      <c r="B128" s="22"/>
+      <c r="C128" s="19"/>
+      <c r="D128" s="32"/>
+      <c r="E128" s="32"/>
+      <c r="F128" s="32"/>
+      <c r="G128" s="33"/>
+    </row>
+    <row r="129" spans="1:7">
+      <c r="A129" s="28"/>
+      <c r="B129" s="23"/>
+      <c r="C129" s="24"/>
+      <c r="D129" s="25"/>
+      <c r="E129" s="25"/>
+      <c r="F129" s="25"/>
+      <c r="G129" s="26"/>
     </row>
   </sheetData>
   <mergeCells count="3">

</xml_diff>

<commit_message>
3.0.13: Add queryAndHash property to MenuItemInterface.
</commit_message>
<xml_diff>
--- a/meta/program/BlancoVueComponentResourceBundle.xlsx
+++ b/meta/program/BlancoVueComponentResourceBundle.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tueda/data/webstorm/blanco/blancoVueComponent/meta/program/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE957C3A-CADD-F64C-8C7C-05A8255A937A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA206BB5-D783-EC4C-A9F8-09337DE3AF4C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="6660" yWindow="10080" windowWidth="28800" windowHeight="17540" tabRatio="860" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="178">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="180">
   <si>
     <t>説明</t>
     <rPh sb="0" eb="2">
@@ -981,6 +981,23 @@
     <t>メニューノードの子階層です。</t>
     <rPh sb="8" eb="11">
       <t xml:space="preserve">コカイソウ </t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>XML2SOURCE_FILE.MENU.ITEM.QUERY.AND.HASH</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>メニューノードから遷移する際に付加するQueryとHash文字列です。</t>
+    <rPh sb="9" eb="11">
+      <t xml:space="preserve">センイ </t>
+    </rPh>
+    <rPh sb="15" eb="17">
+      <t xml:space="preserve">フカ </t>
+    </rPh>
+    <rPh sb="29" eb="32">
+      <t xml:space="preserve">モジレツ </t>
     </rPh>
     <phoneticPr fontId="1"/>
   </si>
@@ -1914,10 +1931,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:I129"/>
+  <dimension ref="A1:I130"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A79" workbookViewId="0">
-      <selection activeCell="C114" sqref="C114"/>
+      <selection activeCell="C116" sqref="C116"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14"/>
@@ -3040,7 +3057,7 @@
     </row>
     <row r="81" spans="1:7">
       <c r="A81" s="27">
-        <f t="shared" ref="A81:A127" si="1">A80+1</f>
+        <f t="shared" ref="A81:A128" si="1">A80+1</f>
         <v>67</v>
       </c>
       <c r="B81" s="22" t="s">
@@ -3540,8 +3557,8 @@
     </row>
     <row r="113" spans="1:7">
       <c r="A113" s="27">
-        <f>A110+1</f>
-        <v>97</v>
+        <f>A109+1</f>
+        <v>96</v>
       </c>
       <c r="B113" s="22" t="s">
         <v>176</v>
@@ -3556,14 +3573,14 @@
     </row>
     <row r="114" spans="1:7">
       <c r="A114" s="27">
-        <f>A111+1</f>
-        <v>98</v>
+        <f>A110+1</f>
+        <v>97</v>
       </c>
       <c r="B114" s="22" t="s">
-        <v>174</v>
+        <v>178</v>
       </c>
       <c r="C114" s="19" t="s">
-        <v>175</v>
+        <v>179</v>
       </c>
       <c r="D114" s="20"/>
       <c r="E114" s="20"/>
@@ -3572,11 +3589,15 @@
     </row>
     <row r="115" spans="1:7">
       <c r="A115" s="27">
-        <f t="shared" si="1"/>
-        <v>99</v>
-      </c>
-      <c r="B115" s="22"/>
-      <c r="C115" s="19"/>
+        <f>A111+1</f>
+        <v>98</v>
+      </c>
+      <c r="B115" s="22" t="s">
+        <v>174</v>
+      </c>
+      <c r="C115" s="19" t="s">
+        <v>175</v>
+      </c>
       <c r="D115" s="20"/>
       <c r="E115" s="20"/>
       <c r="F115" s="20"/>
@@ -3585,7 +3606,7 @@
     <row r="116" spans="1:7">
       <c r="A116" s="27">
         <f t="shared" si="1"/>
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B116" s="22"/>
       <c r="C116" s="19"/>
@@ -3597,12 +3618,10 @@
     <row r="117" spans="1:7">
       <c r="A117" s="27">
         <f t="shared" si="1"/>
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B117" s="22"/>
-      <c r="C117" s="19" t="s">
-        <v>69</v>
-      </c>
+      <c r="C117" s="19"/>
       <c r="D117" s="20"/>
       <c r="E117" s="20"/>
       <c r="F117" s="20"/>
@@ -3611,11 +3630,11 @@
     <row r="118" spans="1:7">
       <c r="A118" s="27">
         <f t="shared" si="1"/>
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B118" s="22"/>
       <c r="C118" s="19" t="s">
-        <v>85</v>
+        <v>69</v>
       </c>
       <c r="D118" s="20"/>
       <c r="E118" s="20"/>
@@ -3625,11 +3644,11 @@
     <row r="119" spans="1:7">
       <c r="A119" s="27">
         <f t="shared" si="1"/>
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B119" s="22"/>
       <c r="C119" s="19" t="s">
-        <v>69</v>
+        <v>85</v>
       </c>
       <c r="D119" s="20"/>
       <c r="E119" s="20"/>
@@ -3639,13 +3658,11 @@
     <row r="120" spans="1:7">
       <c r="A120" s="27">
         <f t="shared" si="1"/>
-        <v>104</v>
-      </c>
-      <c r="B120" s="22" t="s">
-        <v>91</v>
-      </c>
+        <v>103</v>
+      </c>
+      <c r="B120" s="22"/>
       <c r="C120" s="19" t="s">
-        <v>92</v>
+        <v>69</v>
       </c>
       <c r="D120" s="20"/>
       <c r="E120" s="20"/>
@@ -3655,13 +3672,13 @@
     <row r="121" spans="1:7">
       <c r="A121" s="27">
         <f t="shared" si="1"/>
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B121" s="22" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C121" s="19" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="D121" s="20"/>
       <c r="E121" s="20"/>
@@ -3671,13 +3688,13 @@
     <row r="122" spans="1:7">
       <c r="A122" s="27">
         <f t="shared" si="1"/>
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B122" s="22" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C122" s="19" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="D122" s="20"/>
       <c r="E122" s="20"/>
@@ -3687,13 +3704,13 @@
     <row r="123" spans="1:7">
       <c r="A123" s="27">
         <f t="shared" si="1"/>
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B123" s="22" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C123" s="19" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="D123" s="20"/>
       <c r="E123" s="20"/>
@@ -3703,13 +3720,13 @@
     <row r="124" spans="1:7">
       <c r="A124" s="27">
         <f t="shared" si="1"/>
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B124" s="22" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C124" s="19" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="D124" s="20"/>
       <c r="E124" s="20"/>
@@ -3719,13 +3736,13 @@
     <row r="125" spans="1:7">
       <c r="A125" s="27">
         <f t="shared" si="1"/>
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B125" s="22" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C125" s="19" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="D125" s="20"/>
       <c r="E125" s="20"/>
@@ -3735,13 +3752,13 @@
     <row r="126" spans="1:7">
       <c r="A126" s="27">
         <f t="shared" si="1"/>
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B126" s="22" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C126" s="19" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="D126" s="20"/>
       <c r="E126" s="20"/>
@@ -3751,13 +3768,13 @@
     <row r="127" spans="1:7">
       <c r="A127" s="27">
         <f t="shared" si="1"/>
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B127" s="22" t="s">
-        <v>86</v>
+        <v>103</v>
       </c>
       <c r="C127" s="19" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D127" s="20"/>
       <c r="E127" s="20"/>
@@ -3765,22 +3782,38 @@
       <c r="G127" s="21"/>
     </row>
     <row r="128" spans="1:7">
-      <c r="A128" s="27"/>
-      <c r="B128" s="22"/>
-      <c r="C128" s="19"/>
-      <c r="D128" s="32"/>
-      <c r="E128" s="32"/>
-      <c r="F128" s="32"/>
-      <c r="G128" s="33"/>
+      <c r="A128" s="27">
+        <f t="shared" si="1"/>
+        <v>111</v>
+      </c>
+      <c r="B128" s="22" t="s">
+        <v>86</v>
+      </c>
+      <c r="C128" s="19" t="s">
+        <v>105</v>
+      </c>
+      <c r="D128" s="20"/>
+      <c r="E128" s="20"/>
+      <c r="F128" s="20"/>
+      <c r="G128" s="21"/>
     </row>
     <row r="129" spans="1:7">
-      <c r="A129" s="28"/>
-      <c r="B129" s="23"/>
-      <c r="C129" s="24"/>
-      <c r="D129" s="25"/>
-      <c r="E129" s="25"/>
-      <c r="F129" s="25"/>
-      <c r="G129" s="26"/>
+      <c r="A129" s="27"/>
+      <c r="B129" s="22"/>
+      <c r="C129" s="19"/>
+      <c r="D129" s="32"/>
+      <c r="E129" s="32"/>
+      <c r="F129" s="32"/>
+      <c r="G129" s="33"/>
+    </row>
+    <row r="130" spans="1:7">
+      <c r="A130" s="28"/>
+      <c r="B130" s="23"/>
+      <c r="C130" s="24"/>
+      <c r="D130" s="25"/>
+      <c r="E130" s="25"/>
+      <c r="F130" s="25"/>
+      <c r="G130" s="26"/>
     </row>
   </sheetData>
   <mergeCells count="3">

</xml_diff>